<commit_message>
Js ToDo List exe file updated
</commit_message>
<xml_diff>
--- a/JsToDoList/ToDoLearning.xlsx
+++ b/JsToDoList/ToDoLearning.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="9405"/>
+    <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="9405" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="JavaScript" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="319">
   <si>
     <t>Date</t>
   </si>
@@ -882,6 +882,187 @@
     <t>The filter() method creates a new array filled with elements that pass a test provided by a function. 
 The filter() method does not execute the function for empty elements. 
 The filter() method does not change the original array.</t>
+  </si>
+  <si>
+    <t>The sort() method can be used to sort elements of an array in ascending order based on Unicode character code values by default</t>
+  </si>
+  <si>
+    <t>JavaScript reduce() is a higher order function used in data manipulation that reduces an array to a single value. It takes two parameters: an accumulator and the current element of an array.</t>
+  </si>
+  <si>
+    <t>The includes() method returns true if a string contains a specified string. Otherwise it returns false . The includes() method is case sensitive.</t>
+  </si>
+  <si>
+    <t>The every() method executes a function for each array element. 
+The every() method returns true if the function returns true for all elements. 
+The every() method returns false if the function returns false for one element.</t>
+  </si>
+  <si>
+    <t>The some() method executes the callback function once for each array element. The some() method returns true (and stops) if the function returns true for one of the array elements.</t>
+  </si>
+  <si>
+    <t>The find() method returns the value of the first element that passes a test. 
+The find() method executes a function for each array element. 
+The find() method returns undefined if no elements are found.</t>
+  </si>
+  <si>
+    <t>The split() method splits a string into an array of substrings. 
+The split() method returns the new array. 
+The split() method does not change the original string. If (" ") is used as separator, the string is split between words.</t>
+  </si>
+  <si>
+    <t>The splice() method is used to add or remove elements of an existing array and the return value will be the removed items from the array.
+ If nothing was removed from the array, then the return value will just be an empty array.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The slice() method extracts a part of a string. 
+The slice() method returns the extracted part in a new string. 
+The slice() method does not change the original string. 
+The start and end parameters specifies the part of the string to extract. </t>
+  </si>
+  <si>
+    <t>The push() method adds new items to the end of an array. 
+The push() method changes the length of the array. 
+The push() method returns the new length.</t>
+  </si>
+  <si>
+    <t>The pop() method removes (pops) the last element of an array. 
+The pop() method changes the original array. 
+The pop() method returns the removed element.</t>
+  </si>
+  <si>
+    <t>The shift() method removes the first item of an array. 
+The shift() method changes the original array. 
+The shift() method returns the shifted element.</t>
+  </si>
+  <si>
+    <t>The unshift() method adds new elements to the beginning of an array. 
+The unshift() method overwrites the original array.</t>
+  </si>
+  <si>
+    <t>The concat() method concatenates (joins) two or more arrays. 
+The concat() method returns a new array, containing the joined arrays.</t>
+  </si>
+  <si>
+    <t>The spread operator ( ... ) helps you expand iterables into individual elements</t>
+  </si>
+  <si>
+    <t>Iteration occurs when we want to execute code once for each item in a collection, usually elements in an array or properties of an object.</t>
+  </si>
+  <si>
+    <t>The constructor is a method used to initialize an object's state in a class. It automatically called during the creation of an object in a class. The concept of a constructor is the same in React. The constructor in a React component is called before the component is mounted.</t>
+  </si>
+  <si>
+    <t>Super() function is to call the constructor of the parent class. It is used when we need to access a few variables in the parent class. It returns an object which represents the parent class.</t>
+  </si>
+  <si>
+    <t>The state is a built-in React object that is used to contain data or information about the component. A component's state can change over time; whenever it changes, the component re-renders.</t>
+  </si>
+  <si>
+    <t>Props stand for "Properties." They are read-only components. It is an object which stores the value of attributes of a tag and work similar to the HTML attributes. It gives a way to pass data from one component to other components. It is similar to function arguments.</t>
+  </si>
+  <si>
+    <t>Render is the technique that can redirect a page with the help of function render()</t>
+  </si>
+  <si>
+    <t>components have a lifecycle that consists of different phases. Each phase has a set of lifecycle methods that are called at specific points in the component's lifecycle. These methods allow you to control the component's behavior and perform specific actions at different stages of its lifecycle.</t>
+  </si>
+  <si>
+    <t>There are three categories of lifecycle methods: mounting, updating, and unmounting. A component “mounts” when it renders for the first time. This is when mounting lifecycle methods get called. The first time that a component instance renders, it does not update.</t>
+  </si>
+  <si>
+    <t>The three phases are: Mounting, Updating, and Unmounting.</t>
+  </si>
+  <si>
+    <t>React Reconciliation is the process through which React updates the Browser DOM. It makes the DOM updates faster in React. It updates the virtual DOM first and then uses the diffing algorithm to make efficient and optimized updates in the Real DOM</t>
+  </si>
+  <si>
+    <t>ReactJS Profilers is a tool for profiling the react components, It measures how many times the react Application is rendered and how much time the components take to be rendered.</t>
+  </si>
+  <si>
+    <t>Web Vitals is a set of metrics that measure real-world user experience for loading performance, interactivity, and visual stability of the page</t>
+  </si>
+  <si>
+    <t>An application manifest is a [ JSON ] document that contains startup parameters and application defaults for when a web application is launched</t>
+  </si>
+  <si>
+    <t>Client-side rendering (CSR) is the process of rendering web pages on the client using JavaScript. In this approach, the server sends the initial HTML file, but the client then uses JavaScript to dynamically update the page as needed.</t>
+  </si>
+  <si>
+    <t>Server Side Rendering (SSR) is used to render web pages on the server before sending them to the client. This allows for faster page loads, improved performance, and an SEO-friendly rendering solution for React applications.</t>
+  </si>
+  <si>
+    <t>Your event handlers will be passed instances of SyntheticEvent , a cross-browser wrapper around the browser's native event. It has the same interface as the browser's native event, including stopPropagation() and preventDefault() , except the events work identically across all browsers.</t>
+  </si>
+  <si>
+    <t>The virtual DOM (VDOM) is a programming concept where an ideal, or “virtual”, representation of a UI is kept in memory and synced with the “real” DOM by a library such as ReactDOM.</t>
+  </si>
+  <si>
+    <t>DOM stands for 'Document Object Model'. It is a structured representation of HTML in the webpage or application.
+It represents the entire UI(User Interface) of the web application as the tree data structure. 
+It is a structural representation of HTML elements of a web application in simple words.</t>
+  </si>
+  <si>
+    <t>JSX stands for JavaScript XML. JSX allows us to write HTML in React. JSX makes it easier to write and add HTML in React.</t>
+  </si>
+  <si>
+    <t>Lists are used to display data in an ordered format and mainly used to display menus on websites.</t>
+  </si>
+  <si>
+    <t>A “key” is a special string attribute you need to include when creating lists of elements in React. 
+Keys are used in React to identify which items in the list are changed, updated, or deleted. Keys are used to give an identity to the elements in the lists.</t>
+  </si>
+  <si>
+    <t>Webpack in react is a JavaScript module bundler that is commonly used with React to bundle and manage dependencies. It takes all of the individual JavaScript files and other assets in a project, such as images and CSS, and combines them into a single bundle that can be loaded by the browser.</t>
+  </si>
+  <si>
+    <t>Babel is a JavaScript compiler that converts modern JavaScript code into a version compatible with all browsers. 
+Babel enables React developers to use the latest JavaScript syntax in their components. Babel transpiles modern JavaScript for use in React components and all browsers.</t>
+  </si>
+  <si>
+    <t>The main goal for Karma is to bring a productive testing environment to developers. The environment being one where they don't have to set up loads of configurations, but rather a place where developers can just write the code and get instant feedback from their tests.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hooks are functions that let you “hook into” React state and lifecycle features from function components. Hooks don't work inside classes — they let you use React without classes. </t>
+  </si>
+  <si>
+    <t>useState is React Hook that allows you to add state to a functional component. It returns an array with two values: the current state and a function to update it. The Hook takes an initial state value as an argument and returns an updated state value whenever the setter function is called.</t>
+  </si>
+  <si>
+    <t>The useEffect Hook allows you to perform side effects in your components. Some examples of side effects are: fetching data, directly updating the DOM, and timers.</t>
+  </si>
+  <si>
+    <t>The useReducer Hook is used to store and update states, just like the useState Hook. It accepts a reducer function as its first parameter and the initial state as the second. useReducer returns an array that holds the current state value and a dispatch function to which you can pass an action and later invoke it</t>
+  </si>
+  <si>
+    <t>The useLayoutEffect hook is similar to the useEffect theme in that it fires synchronously once all DOM loading is completed, rather than asynchronous like the useEffect hook. This can be used to re-render the DOM and read its layout concurrently.</t>
+  </si>
+  <si>
+    <t>The useRef Hook allows you to persist values between renders. It can be used to store a mutable value that does not cause a re-render when updated. It can be used to access a DOM element directly.</t>
+  </si>
+  <si>
+    <t>Custom Hooks are a mechanism to reuse stateful logic (such as setting up a subscription and remembering the current value), but every time you use a custom Hook, all state and effects inside of it are fully isolated.</t>
+  </si>
+  <si>
+    <t>By using memo , you are telling React that your component complies with this requirement, so React doesn't need to re-render as long as its props haven't changed. Even with memo , your component will re-render if its own state changes or if a context that it's using changes.</t>
+  </si>
+  <si>
+    <t>useMemo Hook returns a memoized value. Think of memoization as caching a value so that it does not need to be recalculated. The useMemo Hook only runs when one of its dependencies update. This can improve performance. The useMemo and useCallback Hooks are similar.</t>
+  </si>
+  <si>
+    <t>The useCallback hook is a powerful tool that can be used to improve the performance of React components. By memoizing callback functions, useCallback can prevent unnecessary re-renders, which can lead to a smoother user experience</t>
+  </si>
+  <si>
+    <t>Prop drilling occurs when a parent component generates its state and passes it down as props to its children components that do not consume the props – instead, they only pass it down to another component that finally consumes it.</t>
+  </si>
+  <si>
+    <t>Context API allows data to be passed through a component tree without having to pass props manually at every level. This makes it easier to share data between components.</t>
+  </si>
+  <si>
+    <t>useContext is a React hook that provides a way to share data (context) across multiple components without explicitly passing it through props. It is part of the React Context API, which is built into the React library.</t>
+  </si>
+  <si>
+    <t>createContext returns a context object. The context object itself does not hold any information. It represents which context other components read or provide. Typically, you will use SomeContext.Provider in components above to specify the context value, and call useContext(SomeContext) in components below to read it.</t>
   </si>
 </sst>
 </file>
@@ -990,7 +1171,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1009,8 +1190,20 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor rgb="FF0B5394"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1033,11 +1226,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -1102,6 +1304,35 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1319,9 +1550,9 @@
   </sheetPr>
   <dimension ref="A1:I209"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C33" sqref="C33"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1685,119 +1916,151 @@
       </c>
       <c r="D33" s="29"/>
     </row>
-    <row r="34" spans="2:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:5" ht="31.5" x14ac:dyDescent="0.2">
       <c r="B34" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="C34" s="29"/>
+      <c r="C34" s="29" t="s">
+        <v>266</v>
+      </c>
       <c r="D34" s="29"/>
     </row>
-    <row r="35" spans="2:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:5" ht="47.25" x14ac:dyDescent="0.2">
       <c r="B35" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="C35" s="29"/>
+      <c r="C35" s="29" t="s">
+        <v>267</v>
+      </c>
       <c r="D35" s="29"/>
     </row>
-    <row r="36" spans="2:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:5" ht="31.5" x14ac:dyDescent="0.2">
       <c r="B36" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="C36" s="29"/>
+      <c r="C36" s="29" t="s">
+        <v>268</v>
+      </c>
       <c r="D36" s="29"/>
     </row>
-    <row r="37" spans="2:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:5" ht="47.25" x14ac:dyDescent="0.2">
       <c r="B37" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="C37" s="29"/>
+      <c r="C37" s="29" t="s">
+        <v>269</v>
+      </c>
       <c r="D37" s="29"/>
     </row>
-    <row r="38" spans="2:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:5" ht="47.25" x14ac:dyDescent="0.2">
       <c r="B38" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="C38" s="29"/>
+      <c r="C38" s="29" t="s">
+        <v>270</v>
+      </c>
       <c r="D38" s="29"/>
     </row>
-    <row r="39" spans="2:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:5" ht="47.25" x14ac:dyDescent="0.2">
       <c r="B39" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="C39" s="29"/>
+      <c r="C39" s="29" t="s">
+        <v>271</v>
+      </c>
       <c r="D39" s="29"/>
     </row>
-    <row r="40" spans="2:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:5" ht="63" x14ac:dyDescent="0.2">
       <c r="B40" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="C40" s="29"/>
+      <c r="C40" s="29" t="s">
+        <v>272</v>
+      </c>
       <c r="D40" s="29"/>
     </row>
-    <row r="41" spans="2:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:5" ht="63" x14ac:dyDescent="0.2">
       <c r="B41" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="C41" s="29"/>
+      <c r="C41" s="29" t="s">
+        <v>273</v>
+      </c>
       <c r="D41" s="29"/>
       <c r="E41" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="42" spans="2:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:5" ht="63" x14ac:dyDescent="0.2">
       <c r="B42" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="C42" s="29"/>
+      <c r="C42" s="29" t="s">
+        <v>274</v>
+      </c>
       <c r="D42" s="29"/>
     </row>
-    <row r="43" spans="2:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:5" ht="47.25" x14ac:dyDescent="0.2">
       <c r="B43" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="C43" s="29"/>
+      <c r="C43" s="29" t="s">
+        <v>275</v>
+      </c>
       <c r="D43" s="29"/>
     </row>
-    <row r="44" spans="2:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:5" ht="47.25" x14ac:dyDescent="0.2">
       <c r="B44" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="C44" s="29"/>
+      <c r="C44" s="29" t="s">
+        <v>276</v>
+      </c>
       <c r="D44" s="29"/>
     </row>
-    <row r="45" spans="2:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:5" ht="47.25" x14ac:dyDescent="0.2">
       <c r="B45" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="C45" s="29"/>
+      <c r="C45" s="29" t="s">
+        <v>277</v>
+      </c>
       <c r="D45" s="29"/>
     </row>
-    <row r="46" spans="2:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:5" ht="31.5" x14ac:dyDescent="0.2">
       <c r="B46" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="C46" s="29"/>
+      <c r="C46" s="29" t="s">
+        <v>278</v>
+      </c>
       <c r="D46" s="29"/>
     </row>
-    <row r="47" spans="2:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:5" ht="31.5" x14ac:dyDescent="0.2">
       <c r="B47" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="C47" s="29"/>
+      <c r="C47" s="29" t="s">
+        <v>279</v>
+      </c>
       <c r="D47" s="29"/>
     </row>
     <row r="48" spans="2:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B48" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="C48" s="26"/>
+      <c r="C48" s="26" t="s">
+        <v>280</v>
+      </c>
       <c r="D48" s="26"/>
     </row>
-    <row r="49" spans="2:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:5" ht="31.5" x14ac:dyDescent="0.2">
       <c r="B49" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="C49" s="26"/>
+      <c r="C49" s="26" t="s">
+        <v>281</v>
+      </c>
       <c r="D49" s="26"/>
     </row>
     <row r="50" spans="2:5" ht="15" x14ac:dyDescent="0.2">
@@ -2548,13 +2811,15 @@
   </sheetPr>
   <dimension ref="A1:H175"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" style="34" customWidth="1"/>
+    <col min="3" max="3" width="76.7109375" style="38" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
     <col min="5" max="5" width="28.28515625" customWidth="1"/>
     <col min="6" max="6" width="30.42578125" customWidth="1"/>
@@ -2562,532 +2827,723 @@
     <col min="8" max="8" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="41"/>
+      <c r="D1" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="39" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>45146</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="32" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="37" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>45148</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="32" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="37" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>45150</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="32" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="37" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>45152</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="32" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="37" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>45154</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="32" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="37" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>45156</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="32" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="37" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>45158</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="32" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="37" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="32" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="37" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>45161</v>
       </c>
-      <c r="B10" s="11"/>
-    </row>
-    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="33"/>
+      <c r="C10" s="37"/>
+    </row>
+    <row r="11" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>45162</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="32" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="37" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>45164</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="32" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="37" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>45166</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="32" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="37" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>45168</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="32" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="37" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>45169</v>
       </c>
-      <c r="B15" s="11"/>
-    </row>
-    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="10" t="s">
+      <c r="B15" s="33"/>
+      <c r="C15" s="37"/>
+    </row>
+    <row r="16" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B16" s="32" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="17" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="10" t="s">
+      <c r="C16" s="37" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B17" s="32" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="18" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="12"/>
-    </row>
-    <row r="19" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="10" t="s">
+      <c r="C17" s="37" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="B18" s="33"/>
+      <c r="C18" s="37"/>
+    </row>
+    <row r="19" spans="2:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="B19" s="32" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="20" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="10" t="s">
+      <c r="C19" s="37" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B20" s="32" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="21" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="10" t="s">
+      <c r="C20" s="37" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="B21" s="32" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="22" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="10" t="s">
+      <c r="C21" s="37" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B22" s="32" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="23" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="10" t="s">
+      <c r="C22" s="37" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B23" s="32" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" s="10" t="s">
+      <c r="C23" s="37" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="B24" s="32" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="25" spans="2:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="B25" s="11"/>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B26" s="10" t="s">
+      <c r="C24" s="37" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="B25" s="33"/>
+      <c r="C25" s="37"/>
+    </row>
+    <row r="26" spans="2:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="B26" s="32" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B27" s="10" t="s">
+      <c r="C26" s="37" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="B27" s="32" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B28" s="10" t="s">
+      <c r="C27" s="37" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B28" s="32" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B29" s="10" t="s">
+      <c r="C28" s="37"/>
+    </row>
+    <row r="29" spans="2:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="B29" s="32" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="30" spans="2:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="B30" s="11"/>
-    </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B31" s="10" t="s">
+      <c r="C29" s="37" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="B30" s="33"/>
+      <c r="C30" s="37"/>
+    </row>
+    <row r="31" spans="2:3" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B31" s="32" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B32" s="10" t="s">
+      <c r="C31" s="37" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="B32" s="32" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="10" t="s">
+      <c r="C32" s="37" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B33" s="32" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="10" t="s">
+      <c r="C33" s="37" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="B34" s="32" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="35" spans="2:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="B35" s="13" t="s">
+      <c r="C34" s="37" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B35" s="33" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B36" s="10" t="s">
+      <c r="C35" s="37" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B36" s="32" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B37" s="10" t="s">
+      <c r="C36" s="37" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B37" s="32" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="38" spans="2:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="B38" s="12"/>
-    </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B39" s="10" t="s">
+      <c r="C37" s="37" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="B38" s="33"/>
+      <c r="C38" s="37"/>
+    </row>
+    <row r="39" spans="2:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="B39" s="32" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B40" s="10" t="s">
+      <c r="C39" s="37" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="B40" s="32" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B41" s="10" t="s">
+      <c r="C40" s="37" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B41" s="32" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B42" s="10" t="s">
+      <c r="C41" s="37" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B42" s="32" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B43" s="10"/>
-    </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B44" s="10" t="s">
+      <c r="C42" s="37"/>
+    </row>
+    <row r="43" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B43" s="32"/>
+      <c r="C43" s="37"/>
+    </row>
+    <row r="44" spans="2:3" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B44" s="32" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B45" s="10" t="s">
+      <c r="C44" s="37" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B45" s="32" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B46" s="10" t="s">
+      <c r="C45" s="37" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B46" s="32" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B47" s="10" t="s">
+      <c r="C46" s="37" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="B47" s="32" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B48" s="10" t="s">
+      <c r="C47" s="37" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B48" s="32" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B49" s="10" t="s">
+      <c r="C48" s="37"/>
+    </row>
+    <row r="49" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B49" s="32" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B50" s="10" t="s">
+      <c r="C49" s="37"/>
+    </row>
+    <row r="50" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B50" s="32" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B51" s="10" t="s">
+      <c r="C50" s="37"/>
+    </row>
+    <row r="51" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B51" s="32" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="52" spans="2:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="B52" s="12"/>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B53" s="10" t="s">
+      <c r="C51" s="37"/>
+    </row>
+    <row r="52" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="B52" s="33"/>
+      <c r="C52" s="37"/>
+    </row>
+    <row r="53" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B53" s="32" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="54" spans="2:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="B54" s="13" t="s">
+      <c r="C53" s="37"/>
+    </row>
+    <row r="54" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="B54" s="33" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B55" s="10" t="s">
+      <c r="C54" s="37"/>
+    </row>
+    <row r="55" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B55" s="32" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="56" spans="2:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="B56" s="13" t="s">
+      <c r="C55" s="37"/>
+    </row>
+    <row r="56" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="B56" s="33" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B57" s="10" t="s">
+      <c r="C56" s="37"/>
+    </row>
+    <row r="57" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B57" s="32" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B58" s="10" t="s">
+      <c r="C57" s="37"/>
+    </row>
+    <row r="58" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B58" s="32" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="59" spans="2:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="B59" s="11"/>
-    </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B60" s="10" t="s">
+      <c r="C58" s="37"/>
+    </row>
+    <row r="59" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="B59" s="33"/>
+      <c r="C59" s="37"/>
+    </row>
+    <row r="60" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B60" s="32" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B61" s="10" t="s">
+      <c r="C60" s="37"/>
+    </row>
+    <row r="61" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B61" s="32" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B62" s="10" t="s">
+      <c r="C61" s="37"/>
+    </row>
+    <row r="62" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B62" s="32" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B63" s="10" t="s">
+      <c r="C62" s="37"/>
+    </row>
+    <row r="63" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B63" s="32" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="64" spans="2:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="B64" s="11"/>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B65" s="10" t="s">
+      <c r="C63" s="37"/>
+    </row>
+    <row r="64" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="B64" s="33"/>
+      <c r="C64" s="37"/>
+    </row>
+    <row r="65" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B65" s="32" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B66" s="10" t="s">
+      <c r="C65" s="37"/>
+    </row>
+    <row r="66" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B66" s="32" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B67" s="10" t="s">
+      <c r="C66" s="37"/>
+    </row>
+    <row r="67" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B67" s="32" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B70" s="4"/>
-    </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B71" s="4"/>
-    </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B72" s="4"/>
-    </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B73" s="4"/>
-    </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B74" s="4"/>
-    </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B75" s="4"/>
-    </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B76" s="4"/>
-    </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B77" s="4"/>
-    </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B78" s="4"/>
-    </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B79" s="4"/>
-    </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B80" s="4"/>
-    </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B81" s="4"/>
-    </row>
-    <row r="83" spans="2:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="B83" s="5"/>
-    </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B84" s="4"/>
-    </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B85" s="4"/>
-    </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B86" s="4"/>
-    </row>
-    <row r="87" spans="2:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="B87" s="8"/>
-    </row>
-    <row r="89" spans="2:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="B89" s="5"/>
-    </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B90" s="4"/>
-    </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B91" s="4"/>
-    </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B92" s="4"/>
-    </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B93" s="4"/>
-    </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B94" s="4"/>
-    </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B95" s="4"/>
-    </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B96" s="4"/>
-    </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B97" s="4"/>
-    </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B98" s="4"/>
-    </row>
-    <row r="99" spans="2:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="B99" s="5"/>
-    </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B100" s="4"/>
-    </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B101" s="4"/>
-    </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B102" s="4"/>
-    </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B103" s="4"/>
-    </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B104" s="4"/>
-    </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B105" s="4"/>
-    </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B106" s="4"/>
-    </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B107" s="4"/>
-    </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B108" s="4"/>
-    </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B109" s="4"/>
-    </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B110" s="4"/>
-    </row>
-    <row r="111" spans="2:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="B111" s="5"/>
-    </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B112" s="4"/>
-    </row>
-    <row r="113" spans="2:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="B113" s="5"/>
-    </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B114" s="4"/>
-    </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B115" s="4"/>
-    </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B116" s="4"/>
-    </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B117" s="4"/>
-    </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B118" s="4"/>
-    </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B119" s="4"/>
-    </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B120" s="4"/>
-    </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B121" s="4"/>
-    </row>
-    <row r="175" spans="2:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="B175" s="5"/>
+      <c r="C67" s="37"/>
+    </row>
+    <row r="70" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B70" s="35"/>
+      <c r="C70" s="37"/>
+    </row>
+    <row r="71" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B71" s="35"/>
+      <c r="C71" s="37"/>
+    </row>
+    <row r="72" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B72" s="35"/>
+      <c r="C72" s="37"/>
+    </row>
+    <row r="73" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B73" s="35"/>
+      <c r="C73" s="37"/>
+    </row>
+    <row r="74" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B74" s="35"/>
+      <c r="C74" s="37"/>
+    </row>
+    <row r="75" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B75" s="35"/>
+      <c r="C75" s="37"/>
+    </row>
+    <row r="76" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B76" s="35"/>
+      <c r="C76" s="37"/>
+    </row>
+    <row r="77" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B77" s="35"/>
+      <c r="C77" s="37"/>
+    </row>
+    <row r="78" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B78" s="35"/>
+      <c r="C78" s="37"/>
+    </row>
+    <row r="79" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B79" s="35"/>
+      <c r="C79" s="37"/>
+    </row>
+    <row r="80" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B80" s="35"/>
+      <c r="C80" s="37"/>
+    </row>
+    <row r="81" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B81" s="35"/>
+      <c r="C81" s="37"/>
+    </row>
+    <row r="83" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="B83" s="36"/>
+      <c r="C83" s="37"/>
+    </row>
+    <row r="84" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B84" s="35"/>
+      <c r="C84" s="37"/>
+    </row>
+    <row r="85" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B85" s="35"/>
+      <c r="C85" s="37"/>
+    </row>
+    <row r="86" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B86" s="35"/>
+      <c r="C86" s="37"/>
+    </row>
+    <row r="87" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="B87" s="36"/>
+      <c r="C87" s="37"/>
+    </row>
+    <row r="89" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="B89" s="36"/>
+      <c r="C89" s="37"/>
+    </row>
+    <row r="90" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B90" s="35"/>
+      <c r="C90" s="37"/>
+    </row>
+    <row r="91" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B91" s="35"/>
+      <c r="C91" s="37"/>
+    </row>
+    <row r="92" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B92" s="35"/>
+      <c r="C92" s="37"/>
+    </row>
+    <row r="93" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B93" s="35"/>
+      <c r="C93" s="37"/>
+    </row>
+    <row r="94" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B94" s="35"/>
+      <c r="C94" s="37"/>
+    </row>
+    <row r="95" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B95" s="35"/>
+      <c r="C95" s="37"/>
+    </row>
+    <row r="96" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B96" s="35"/>
+      <c r="C96" s="37"/>
+    </row>
+    <row r="97" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B97" s="35"/>
+      <c r="C97" s="37"/>
+    </row>
+    <row r="98" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B98" s="35"/>
+      <c r="C98" s="37"/>
+    </row>
+    <row r="99" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="B99" s="36"/>
+      <c r="C99" s="37"/>
+    </row>
+    <row r="100" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B100" s="35"/>
+      <c r="C100" s="37"/>
+    </row>
+    <row r="101" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B101" s="35"/>
+      <c r="C101" s="37"/>
+    </row>
+    <row r="102" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B102" s="35"/>
+      <c r="C102" s="37"/>
+    </row>
+    <row r="103" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B103" s="35"/>
+      <c r="C103" s="37"/>
+    </row>
+    <row r="104" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B104" s="35"/>
+      <c r="C104" s="37"/>
+    </row>
+    <row r="105" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B105" s="35"/>
+      <c r="C105" s="37"/>
+    </row>
+    <row r="106" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B106" s="35"/>
+      <c r="C106" s="37"/>
+    </row>
+    <row r="107" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B107" s="35"/>
+      <c r="C107" s="37"/>
+    </row>
+    <row r="108" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B108" s="35"/>
+      <c r="C108" s="37"/>
+    </row>
+    <row r="109" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B109" s="35"/>
+      <c r="C109" s="37"/>
+    </row>
+    <row r="110" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B110" s="35"/>
+      <c r="C110" s="37"/>
+    </row>
+    <row r="111" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="B111" s="36"/>
+      <c r="C111" s="37"/>
+    </row>
+    <row r="112" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B112" s="35"/>
+      <c r="C112" s="37"/>
+    </row>
+    <row r="113" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="B113" s="36"/>
+      <c r="C113" s="37"/>
+    </row>
+    <row r="114" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B114" s="35"/>
+      <c r="C114" s="37"/>
+    </row>
+    <row r="115" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B115" s="35"/>
+      <c r="C115" s="37"/>
+    </row>
+    <row r="116" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B116" s="35"/>
+      <c r="C116" s="37"/>
+    </row>
+    <row r="117" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B117" s="35"/>
+      <c r="C117" s="37"/>
+    </row>
+    <row r="118" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B118" s="35"/>
+      <c r="C118" s="37"/>
+    </row>
+    <row r="119" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B119" s="35"/>
+      <c r="C119" s="37"/>
+    </row>
+    <row r="120" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B120" s="35"/>
+      <c r="C120" s="37"/>
+    </row>
+    <row r="121" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B121" s="35"/>
+      <c r="C121" s="37"/>
+    </row>
+    <row r="175" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="B175" s="36"/>
+      <c r="C175" s="37"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>